<commit_message>
may be last commit
</commit_message>
<xml_diff>
--- a/REPORT/Checklist.xlsx
+++ b/REPORT/Checklist.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project1\REPORT\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7EA624-EAAB-4ED8-AC0A-01CE6B9A2B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,12 +24,112 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t>LÊ VĂN THÀNH ĐẠT - 24120036</t>
+  </si>
+  <si>
+    <t>TRƯƠNG ĐÌNH NHẬT HUY - 24120064</t>
+  </si>
+  <si>
+    <t>Bubble sort</t>
+  </si>
+  <si>
+    <t>Counting sort</t>
+  </si>
+  <si>
+    <t>Heap sort</t>
+  </si>
+  <si>
+    <t>Insertion sort</t>
+  </si>
+  <si>
+    <t>Merge sort</t>
+  </si>
+  <si>
+    <t>Slection sort</t>
+  </si>
+  <si>
+    <t>Shell sort</t>
+  </si>
+  <si>
+    <t>Radix sort</t>
+  </si>
+  <si>
+    <t>Quick sort</t>
+  </si>
+  <si>
+    <t>Flash sort</t>
+  </si>
+  <si>
+    <t>Shaker sort</t>
+  </si>
+  <si>
+    <t>Build read file, write file</t>
+  </si>
+  <si>
+    <t>Build test case</t>
+  </si>
+  <si>
+    <t>Complete main function</t>
+  </si>
+  <si>
+    <t>Build header file</t>
+  </si>
+  <si>
+    <t>Build charts &amp; Report file</t>
+  </si>
+  <si>
+    <t>Testing (16 cases)</t>
+  </si>
+  <si>
+    <t>Build arguments in main</t>
+  </si>
+  <si>
+    <t>Analyzing time complexity</t>
+  </si>
+  <si>
+    <t>Analyzing data size &amp; comparisons</t>
+  </si>
+  <si>
+    <t>https://github.com/BinElvan3126/Project1</t>
+  </si>
+  <si>
+    <t>Our workspace</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -37,7 +143,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -45,14 +151,154 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -66,6 +312,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>12328</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>13196</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>49028</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{039FF710-6AA2-06F4-9A5B-2F44D12AB962}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3626225"/>
+          <a:ext cx="9790328" cy="4575082"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +625,173 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="73.28515625" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
+    </row>
+    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="7"/>
+    </row>
+    <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="9"/>
+    </row>
+    <row r="14" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+    </row>
+    <row r="15" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="A15" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="15"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B23"/>
+    <mergeCell ref="A15:B15"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A16" r:id="rId1" xr:uid="{03AA5927-0581-49E1-ACAF-249D316FF665}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>